<commit_message>
update srs after modifying siq and cr ids
</commit_message>
<xml_diff>
--- a/Requirements/SIQ.xlsx
+++ b/Requirements/SIQ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\coding\Internet-Banking-System\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="204">
   <si>
     <t>ID</t>
   </si>
@@ -760,6 +760,60 @@
 6- phone number in which he will receive verification code sms
 7- staff ID .
                  </t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q46</t>
+  </si>
+  <si>
+    <t>The client shall have button with title accounts
+ in all pages, so he can back to his accounts page 
+from any page.</t>
+  </si>
+  <si>
+    <t>khadija mostafa</t>
+  </si>
+  <si>
+    <t>"10/5/2019"</t>
+  </si>
+  <si>
+    <t>how can customer navigate to his accounts page from any page?</t>
+  </si>
+  <si>
+    <t>Any popup message shall be in the form of pop up with close icon and button with title ok.</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q47</t>
+  </si>
+  <si>
+    <t>how any error message should be dislayed ?</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q48</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q49</t>
+  </si>
+  <si>
+    <t>Login page shall have button with title login and
+ register in the form of hyper link.</t>
+  </si>
+  <si>
+    <t>what is the shape of register and login in the login page ?</t>
+  </si>
+  <si>
+    <t>Register page shall have button with title register and login in the form of hyper link</t>
+  </si>
+  <si>
+    <t>what is the shape of register and login in the registeration page ?</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q50</t>
+  </si>
+  <si>
+    <t>Customer main page shall have button with title show details to be redirected to account page and other button with title previous transaction to be redirected to previous transactions page.</t>
+  </si>
+  <si>
+    <t>what is the shae of customer account page ?</t>
   </si>
 </sst>
 </file>
@@ -898,7 +952,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1025,11 +1079,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1307,7 +1372,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1357,6 +1421,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1669,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AA67"/>
+  <dimension ref="B3:AA71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1690,55 +1766,55 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="111" t="s">
+      <c r="C3" s="110" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="112"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
     </row>
     <row r="6" spans="3:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="112" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="113" t="s">
+      <c r="D7" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="113" t="s">
+      <c r="E7" s="112" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="113" t="s">
+      <c r="F7" s="112" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="107" t="s">
+      <c r="G7" s="106" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="107" t="s">
+      <c r="H7" s="106" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="107" t="s">
+      <c r="I7" s="106" t="s">
         <v>85</v>
       </c>
-      <c r="J7" s="107" t="s">
+      <c r="J7" s="106" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="8" spans="3:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="108"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
     </row>
     <row r="9" spans="3:12" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
@@ -1785,7 +1861,7 @@
       <c r="H10" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I10" s="104">
+      <c r="I10" s="103">
         <v>43501</v>
       </c>
       <c r="J10" s="6" t="s">
@@ -1811,7 +1887,7 @@
       <c r="H11" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="I11" s="103">
+      <c r="I11" s="102">
         <v>43501</v>
       </c>
       <c r="J11" s="90" t="s">
@@ -1829,15 +1905,15 @@
       <c r="J12" s="9"/>
     </row>
     <row r="15" spans="3:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="109" t="s">
+      <c r="C15" s="108" t="s">
         <v>178</v>
       </c>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
     </row>
     <row r="21" spans="2:27" s="53" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="54" t="s">
@@ -2196,7 +2272,7 @@
       <c r="AA28" s="72"/>
     </row>
     <row r="29" spans="2:27" s="1" customFormat="1" ht="153.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="105" t="s">
+      <c r="B29" s="104" t="s">
         <v>116</v>
       </c>
       <c r="C29" s="18" t="s">
@@ -3136,7 +3212,7 @@
       <c r="AA49" s="48"/>
     </row>
     <row r="50" spans="2:27" s="13" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="105" t="s">
+      <c r="B50" s="104" t="s">
         <v>137</v>
       </c>
       <c r="C50" s="41" t="s">
@@ -3487,7 +3563,7 @@
         <v>153</v>
       </c>
       <c r="D59" s="63"/>
-      <c r="E59" s="98" t="s">
+      <c r="E59" s="97" t="s">
         <v>182</v>
       </c>
       <c r="F59" s="35" t="s">
@@ -3514,7 +3590,7 @@
         <v>154</v>
       </c>
       <c r="D60" s="62"/>
-      <c r="E60" s="99" t="s">
+      <c r="E60" s="98" t="s">
         <v>155</v>
       </c>
       <c r="F60" s="35" t="s">
@@ -3537,11 +3613,11 @@
       <c r="B61" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="C61" s="100" t="s">
+      <c r="C61" s="99" t="s">
         <v>156</v>
       </c>
       <c r="D61" s="75"/>
-      <c r="E61" s="100" t="s">
+      <c r="E61" s="99" t="s">
         <v>158</v>
       </c>
       <c r="F61" s="35" t="s">
@@ -3564,7 +3640,7 @@
       <c r="B62" s="65" t="s">
         <v>159</v>
       </c>
-      <c r="C62" s="101" t="s">
+      <c r="C62" s="100" t="s">
         <v>160</v>
       </c>
       <c r="D62" s="84" t="s">
@@ -3591,7 +3667,7 @@
       <c r="B63" s="65" t="s">
         <v>164</v>
       </c>
-      <c r="C63" s="102" t="s">
+      <c r="C63" s="101" t="s">
         <v>163</v>
       </c>
       <c r="D63" s="92"/>
@@ -3616,7 +3692,7 @@
       <c r="B64" s="65" t="s">
         <v>167</v>
       </c>
-      <c r="C64" s="101" t="s">
+      <c r="C64" s="100" t="s">
         <v>165</v>
       </c>
       <c r="D64" s="92"/>
@@ -3641,7 +3717,7 @@
       <c r="B65" s="65" t="s">
         <v>168</v>
       </c>
-      <c r="C65" s="101" t="s">
+      <c r="C65" s="100" t="s">
         <v>166</v>
       </c>
       <c r="D65" s="95"/>
@@ -3663,10 +3739,10 @@
       </c>
     </row>
     <row r="66" spans="2:10" s="82" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="106" t="s">
+      <c r="B66" s="105" t="s">
         <v>172</v>
       </c>
-      <c r="C66" s="101" t="s">
+      <c r="C66" s="100" t="s">
         <v>177</v>
       </c>
       <c r="D66" s="85" t="s">
@@ -3691,8 +3767,150 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D67" s="97"/>
+    <row r="67" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B67" s="105" t="s">
+        <v>187</v>
+      </c>
+      <c r="C67" s="100" t="s">
+        <v>191</v>
+      </c>
+      <c r="D67" s="85" t="s">
+        <v>188</v>
+      </c>
+      <c r="E67" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G67" s="114" t="s">
+        <v>189</v>
+      </c>
+      <c r="H67" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I67" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J67" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B68" s="105" t="s">
+        <v>193</v>
+      </c>
+      <c r="C68" s="100" t="s">
+        <v>194</v>
+      </c>
+      <c r="D68" s="85" t="s">
+        <v>192</v>
+      </c>
+      <c r="E68" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G68" s="114" t="s">
+        <v>189</v>
+      </c>
+      <c r="H68" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I68" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J68" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B69" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="C69" s="115" t="s">
+        <v>198</v>
+      </c>
+      <c r="D69" s="116" t="s">
+        <v>197</v>
+      </c>
+      <c r="E69" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G69" s="114" t="s">
+        <v>189</v>
+      </c>
+      <c r="H69" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I69" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J69" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B70" s="105" t="s">
+        <v>196</v>
+      </c>
+      <c r="C70" s="115" t="s">
+        <v>200</v>
+      </c>
+      <c r="D70" s="116" t="s">
+        <v>199</v>
+      </c>
+      <c r="E70" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G70" s="114" t="s">
+        <v>189</v>
+      </c>
+      <c r="H70" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I70" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J70" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="B71" s="105" t="s">
+        <v>201</v>
+      </c>
+      <c r="C71" s="117" t="s">
+        <v>203</v>
+      </c>
+      <c r="D71" s="116" t="s">
+        <v>202</v>
+      </c>
+      <c r="E71" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G71" s="114" t="s">
+        <v>189</v>
+      </c>
+      <c r="H71" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I71" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J71" s="69" t="s">
+        <v>190</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
update new questions in siq to cover all testcases and update SRS with new requirment according to these questions
</commit_message>
<xml_diff>
--- a/Requirements/SIQ.xlsx
+++ b/Requirements/SIQ.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="225">
   <si>
     <t>ID</t>
   </si>
@@ -814,6 +814,71 @@
   </si>
   <si>
     <t>what is the shae of customer account page ?</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q51</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q52</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q53</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q54</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q55</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q56</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q57</t>
+  </si>
+  <si>
+    <t>Customer shall be redirected to login page with empty fields if customer press on logout hyperlink from his (accounts/ account/previous transaction/ listing) page</t>
+  </si>
+  <si>
+    <t>where shall Customer  be redirected to  if customer press on logout hyperlink from his (accounts/ account/previous transaction/ listing) page</t>
+  </si>
+  <si>
+    <t>If customer press back from his account page, customer shall be redirected to his main/accounts page.</t>
+  </si>
+  <si>
+    <t>If customer press back from his listing page, customer shall be redirected to his previous transaction page.</t>
+  </si>
+  <si>
+    <t>to where shall customer be redirected if he press back from his account page?</t>
+  </si>
+  <si>
+    <t>to where shall customer be redirected if he press back from his listing  page?</t>
+  </si>
+  <si>
+    <t>to where shall customer be redirected if he press back from his previous transaction  page?</t>
+  </si>
+  <si>
+    <t>If customer press back from his previous transactions page, customer shall be redirected to his account  page.</t>
+  </si>
+  <si>
+    <t>The listing page shall have scroll bar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what if the number of the previous transaction page greater than 
+the screen ? 
+</t>
+  </si>
+  <si>
+    <t>If customer click on the login hyper link, customer shall be redirected to login page.</t>
+  </si>
+  <si>
+    <t>to where shall customer be redirected if he click on the login hyper link ? .</t>
+  </si>
+  <si>
+    <t>If customer press on ok button in any pop up message customer shall remain in the same page.</t>
+  </si>
+  <si>
+    <t>what shall happen if the customer press on ok button or close icon for any pp up message ?</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1399,6 +1464,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1423,17 +1500,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1745,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AA71"/>
+  <dimension ref="B3:AA78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="J71" sqref="J71:J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1766,55 +1840,55 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="110" t="s">
+      <c r="C3" s="114" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="111"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
     </row>
     <row r="6" spans="3:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="116" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="112" t="s">
+      <c r="D7" s="116" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="112" t="s">
+      <c r="E7" s="116" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="112" t="s">
+      <c r="F7" s="116" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="106" t="s">
+      <c r="G7" s="110" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="106" t="s">
+      <c r="H7" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="106" t="s">
+      <c r="I7" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="J7" s="106" t="s">
+      <c r="J7" s="110" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="8" spans="3:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="113"/>
-      <c r="D8" s="113"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="113"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="117"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="117"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
     </row>
     <row r="9" spans="3:12" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
@@ -1905,15 +1979,15 @@
       <c r="J12" s="9"/>
     </row>
     <row r="15" spans="3:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="112" t="s">
         <v>178</v>
       </c>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="109"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
     </row>
     <row r="21" spans="2:27" s="53" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="54" t="s">
@@ -3783,7 +3857,7 @@
       <c r="F67" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="G67" s="114" t="s">
+      <c r="G67" s="106" t="s">
         <v>189</v>
       </c>
       <c r="H67" s="35" t="s">
@@ -3812,7 +3886,7 @@
       <c r="F68" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="114" t="s">
+      <c r="G68" s="106" t="s">
         <v>189</v>
       </c>
       <c r="H68" s="35" t="s">
@@ -3829,10 +3903,10 @@
       <c r="B69" s="105" t="s">
         <v>195</v>
       </c>
-      <c r="C69" s="115" t="s">
+      <c r="C69" s="107" t="s">
         <v>198</v>
       </c>
-      <c r="D69" s="116" t="s">
+      <c r="D69" s="108" t="s">
         <v>197</v>
       </c>
       <c r="E69" s="84" t="s">
@@ -3841,7 +3915,7 @@
       <c r="F69" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="G69" s="114" t="s">
+      <c r="G69" s="106" t="s">
         <v>189</v>
       </c>
       <c r="H69" s="35" t="s">
@@ -3858,10 +3932,10 @@
       <c r="B70" s="105" t="s">
         <v>196</v>
       </c>
-      <c r="C70" s="115" t="s">
+      <c r="C70" s="107" t="s">
         <v>200</v>
       </c>
-      <c r="D70" s="116" t="s">
+      <c r="D70" s="108" t="s">
         <v>199</v>
       </c>
       <c r="E70" s="84" t="s">
@@ -3870,7 +3944,7 @@
       <c r="F70" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="G70" s="114" t="s">
+      <c r="G70" s="106" t="s">
         <v>189</v>
       </c>
       <c r="H70" s="35" t="s">
@@ -3887,10 +3961,10 @@
       <c r="B71" s="105" t="s">
         <v>201</v>
       </c>
-      <c r="C71" s="117" t="s">
+      <c r="C71" s="109" t="s">
         <v>203</v>
       </c>
-      <c r="D71" s="116" t="s">
+      <c r="D71" s="108" t="s">
         <v>202</v>
       </c>
       <c r="E71" s="84" t="s">
@@ -3899,7 +3973,7 @@
       <c r="F71" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="G71" s="114" t="s">
+      <c r="G71" s="106" t="s">
         <v>189</v>
       </c>
       <c r="H71" s="35" t="s">
@@ -3909,6 +3983,209 @@
         <v>190</v>
       </c>
       <c r="J71" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="B72" s="105" t="s">
+        <v>204</v>
+      </c>
+      <c r="C72" s="107" t="s">
+        <v>212</v>
+      </c>
+      <c r="D72" s="108" t="s">
+        <v>211</v>
+      </c>
+      <c r="E72" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G72" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H72" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I72" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J72" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B73" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="C73" s="107" t="s">
+        <v>215</v>
+      </c>
+      <c r="D73" s="108" t="s">
+        <v>213</v>
+      </c>
+      <c r="E73" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G73" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H73" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I73" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J73" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B74" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="C74" s="107" t="s">
+        <v>216</v>
+      </c>
+      <c r="D74" s="108" t="s">
+        <v>214</v>
+      </c>
+      <c r="E74" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F74" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G74" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H74" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I74" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J74" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B75" s="105" t="s">
+        <v>207</v>
+      </c>
+      <c r="C75" s="119" t="s">
+        <v>217</v>
+      </c>
+      <c r="D75" s="118" t="s">
+        <v>218</v>
+      </c>
+      <c r="E75" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G75" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H75" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I75" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J75" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B76" s="105" t="s">
+        <v>208</v>
+      </c>
+      <c r="C76" s="107" t="s">
+        <v>220</v>
+      </c>
+      <c r="D76" s="120" t="s">
+        <v>219</v>
+      </c>
+      <c r="E76" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G76" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H76" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I76" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J76" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B77" s="105" t="s">
+        <v>209</v>
+      </c>
+      <c r="C77" s="107" t="s">
+        <v>222</v>
+      </c>
+      <c r="D77" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="E77" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G77" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H77" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I77" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J77" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B78" s="105" t="s">
+        <v>210</v>
+      </c>
+      <c r="C78" s="107" t="s">
+        <v>224</v>
+      </c>
+      <c r="D78" s="120" t="s">
+        <v>223</v>
+      </c>
+      <c r="E78" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F78" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G78" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H78" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I78" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J78" s="69" t="s">
         <v>190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update TCs for registeration and main/ account page and adding some testcases for previoustransaction module
</commit_message>
<xml_diff>
--- a/Requirements/SIQ.xlsx
+++ b/Requirements/SIQ.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="225">
   <si>
     <t>ID</t>
   </si>
@@ -814,6 +814,71 @@
   </si>
   <si>
     <t>what is the shae of customer account page ?</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q51</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q52</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q53</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q54</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q55</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q56</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q57</t>
+  </si>
+  <si>
+    <t>Customer shall be redirected to login page with empty fields if customer press on logout hyperlink from his (accounts/ account/previous transaction/ listing) page</t>
+  </si>
+  <si>
+    <t>where shall Customer  be redirected to  if customer press on logout hyperlink from his (accounts/ account/previous transaction/ listing) page</t>
+  </si>
+  <si>
+    <t>If customer press back from his account page, customer shall be redirected to his main/accounts page.</t>
+  </si>
+  <si>
+    <t>If customer press back from his listing page, customer shall be redirected to his previous transaction page.</t>
+  </si>
+  <si>
+    <t>to where shall customer be redirected if he press back from his account page?</t>
+  </si>
+  <si>
+    <t>to where shall customer be redirected if he press back from his listing  page?</t>
+  </si>
+  <si>
+    <t>to where shall customer be redirected if he press back from his previous transaction  page?</t>
+  </si>
+  <si>
+    <t>If customer press back from his previous transactions page, customer shall be redirected to his account  page.</t>
+  </si>
+  <si>
+    <t>The listing page shall have scroll bar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what if the number of the previous transaction page greater than 
+the screen ? 
+</t>
+  </si>
+  <si>
+    <t>If customer click on the login hyper link, customer shall be redirected to login page.</t>
+  </si>
+  <si>
+    <t>to where shall customer be redirected if he click on the login hyper link ? .</t>
+  </si>
+  <si>
+    <t>If customer press on ok button in any pop up message customer shall remain in the same page.</t>
+  </si>
+  <si>
+    <t>what shall happen if the customer press on ok button or close icon for any pp up message ?</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1399,6 +1464,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1423,17 +1500,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1745,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AA71"/>
+  <dimension ref="B3:AA78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="J71" sqref="J71:J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1766,55 +1840,55 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="110" t="s">
+      <c r="C3" s="114" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="111"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
     </row>
     <row r="6" spans="3:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="116" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="112" t="s">
+      <c r="D7" s="116" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="112" t="s">
+      <c r="E7" s="116" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="112" t="s">
+      <c r="F7" s="116" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="106" t="s">
+      <c r="G7" s="110" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="106" t="s">
+      <c r="H7" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="106" t="s">
+      <c r="I7" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="J7" s="106" t="s">
+      <c r="J7" s="110" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="8" spans="3:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="113"/>
-      <c r="D8" s="113"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="113"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="117"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="117"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
     </row>
     <row r="9" spans="3:12" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
@@ -1905,15 +1979,15 @@
       <c r="J12" s="9"/>
     </row>
     <row r="15" spans="3:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="112" t="s">
         <v>178</v>
       </c>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="109"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
     </row>
     <row r="21" spans="2:27" s="53" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="54" t="s">
@@ -3783,7 +3857,7 @@
       <c r="F67" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="G67" s="114" t="s">
+      <c r="G67" s="106" t="s">
         <v>189</v>
       </c>
       <c r="H67" s="35" t="s">
@@ -3812,7 +3886,7 @@
       <c r="F68" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="114" t="s">
+      <c r="G68" s="106" t="s">
         <v>189</v>
       </c>
       <c r="H68" s="35" t="s">
@@ -3829,10 +3903,10 @@
       <c r="B69" s="105" t="s">
         <v>195</v>
       </c>
-      <c r="C69" s="115" t="s">
+      <c r="C69" s="107" t="s">
         <v>198</v>
       </c>
-      <c r="D69" s="116" t="s">
+      <c r="D69" s="108" t="s">
         <v>197</v>
       </c>
       <c r="E69" s="84" t="s">
@@ -3841,7 +3915,7 @@
       <c r="F69" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="G69" s="114" t="s">
+      <c r="G69" s="106" t="s">
         <v>189</v>
       </c>
       <c r="H69" s="35" t="s">
@@ -3858,10 +3932,10 @@
       <c r="B70" s="105" t="s">
         <v>196</v>
       </c>
-      <c r="C70" s="115" t="s">
+      <c r="C70" s="107" t="s">
         <v>200</v>
       </c>
-      <c r="D70" s="116" t="s">
+      <c r="D70" s="108" t="s">
         <v>199</v>
       </c>
       <c r="E70" s="84" t="s">
@@ -3870,7 +3944,7 @@
       <c r="F70" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="G70" s="114" t="s">
+      <c r="G70" s="106" t="s">
         <v>189</v>
       </c>
       <c r="H70" s="35" t="s">
@@ -3887,10 +3961,10 @@
       <c r="B71" s="105" t="s">
         <v>201</v>
       </c>
-      <c r="C71" s="117" t="s">
+      <c r="C71" s="109" t="s">
         <v>203</v>
       </c>
-      <c r="D71" s="116" t="s">
+      <c r="D71" s="108" t="s">
         <v>202</v>
       </c>
       <c r="E71" s="84" t="s">
@@ -3899,7 +3973,7 @@
       <c r="F71" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="G71" s="114" t="s">
+      <c r="G71" s="106" t="s">
         <v>189</v>
       </c>
       <c r="H71" s="35" t="s">
@@ -3909,6 +3983,209 @@
         <v>190</v>
       </c>
       <c r="J71" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="B72" s="105" t="s">
+        <v>204</v>
+      </c>
+      <c r="C72" s="107" t="s">
+        <v>212</v>
+      </c>
+      <c r="D72" s="108" t="s">
+        <v>211</v>
+      </c>
+      <c r="E72" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G72" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H72" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I72" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J72" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B73" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="C73" s="107" t="s">
+        <v>215</v>
+      </c>
+      <c r="D73" s="108" t="s">
+        <v>213</v>
+      </c>
+      <c r="E73" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G73" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H73" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I73" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J73" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B74" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="C74" s="107" t="s">
+        <v>216</v>
+      </c>
+      <c r="D74" s="108" t="s">
+        <v>214</v>
+      </c>
+      <c r="E74" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F74" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G74" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H74" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I74" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J74" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B75" s="105" t="s">
+        <v>207</v>
+      </c>
+      <c r="C75" s="119" t="s">
+        <v>217</v>
+      </c>
+      <c r="D75" s="118" t="s">
+        <v>218</v>
+      </c>
+      <c r="E75" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G75" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H75" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I75" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J75" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B76" s="105" t="s">
+        <v>208</v>
+      </c>
+      <c r="C76" s="107" t="s">
+        <v>220</v>
+      </c>
+      <c r="D76" s="120" t="s">
+        <v>219</v>
+      </c>
+      <c r="E76" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G76" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H76" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I76" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J76" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B77" s="105" t="s">
+        <v>209</v>
+      </c>
+      <c r="C77" s="107" t="s">
+        <v>222</v>
+      </c>
+      <c r="D77" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="E77" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G77" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H77" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I77" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J77" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B78" s="105" t="s">
+        <v>210</v>
+      </c>
+      <c r="C78" s="107" t="s">
+        <v>224</v>
+      </c>
+      <c r="D78" s="120" t="s">
+        <v>223</v>
+      </c>
+      <c r="E78" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F78" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G78" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H78" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I78" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="J78" s="69" t="s">
         <v>190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating error message in the siq
</commit_message>
<xml_diff>
--- a/Requirements/SIQ.xlsx
+++ b/Requirements/SIQ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\coding\Internet-Banking-System\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\for srs and siq and registeration update\Internet-Banking-System\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="235">
   <si>
     <t>ID</t>
   </si>
@@ -879,6 +879,36 @@
   </si>
   <si>
     <t>what shall happen if the customer press on ok button or close icon for any pp up message ?</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q58</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q59</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q60</t>
+  </si>
+  <si>
+    <t>what is the error message shall be displayed if the customer leave a mandatory field empty ?</t>
+  </si>
+  <si>
+    <t>what is the error message shall be displayed if the customer doesn't achieve length constraint ?</t>
+  </si>
+  <si>
+    <t>what is the error message shall be displayed if the customer doesn't achieve the using chararcters constraints  ?</t>
+  </si>
+  <si>
+    <t>error message beyound the field that " this field is mandatory "</t>
+  </si>
+  <si>
+    <t>error message beyound the field that "length must be between x and y "</t>
+  </si>
+  <si>
+    <t>error message beyound the field that " invalid data format "</t>
+  </si>
+  <si>
+    <t>"18/5/2019"</t>
   </si>
 </sst>
 </file>
@@ -1476,6 +1506,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1499,15 +1538,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1819,10 +1849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AA78"/>
+  <dimension ref="B3:AA81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71:J78"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="J84" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1840,55 +1870,55 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="117" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
     </row>
     <row r="6" spans="3:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="116" t="s">
+      <c r="D7" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="119" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="116" t="s">
+      <c r="F7" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="110" t="s">
+      <c r="G7" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="110" t="s">
+      <c r="H7" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="110" t="s">
+      <c r="I7" s="113" t="s">
         <v>85</v>
       </c>
-      <c r="J7" s="110" t="s">
+      <c r="J7" s="113" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="8" spans="3:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="117"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="117"/>
-      <c r="G8" s="111"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="111"/>
-      <c r="J8" s="111"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="114"/>
     </row>
     <row r="9" spans="3:12" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
@@ -1979,15 +2009,15 @@
       <c r="J12" s="9"/>
     </row>
     <row r="15" spans="3:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="112" t="s">
+      <c r="C15" s="115" t="s">
         <v>178</v>
       </c>
-      <c r="D15" s="113"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="113"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="113"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
+      <c r="G15" s="116"/>
+      <c r="H15" s="116"/>
+      <c r="I15" s="116"/>
     </row>
     <row r="21" spans="2:27" s="53" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="54" t="s">
@@ -4077,10 +4107,10 @@
       <c r="B75" s="105" t="s">
         <v>207</v>
       </c>
-      <c r="C75" s="119" t="s">
+      <c r="C75" s="111" t="s">
         <v>217</v>
       </c>
-      <c r="D75" s="118" t="s">
+      <c r="D75" s="110" t="s">
         <v>218</v>
       </c>
       <c r="E75" s="84" t="s">
@@ -4109,7 +4139,7 @@
       <c r="C76" s="107" t="s">
         <v>220</v>
       </c>
-      <c r="D76" s="120" t="s">
+      <c r="D76" s="112" t="s">
         <v>219</v>
       </c>
       <c r="E76" s="84" t="s">
@@ -4138,7 +4168,7 @@
       <c r="C77" s="107" t="s">
         <v>222</v>
       </c>
-      <c r="D77" s="120" t="s">
+      <c r="D77" s="112" t="s">
         <v>221</v>
       </c>
       <c r="E77" s="84" t="s">
@@ -4167,7 +4197,7 @@
       <c r="C78" s="107" t="s">
         <v>224</v>
       </c>
-      <c r="D78" s="120" t="s">
+      <c r="D78" s="112" t="s">
         <v>223</v>
       </c>
       <c r="E78" s="84" t="s">
@@ -4187,6 +4217,93 @@
       </c>
       <c r="J78" s="69" t="s">
         <v>190</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B79" s="105" t="s">
+        <v>225</v>
+      </c>
+      <c r="C79" s="107" t="s">
+        <v>228</v>
+      </c>
+      <c r="D79" s="112" t="s">
+        <v>231</v>
+      </c>
+      <c r="E79" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F79" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G79" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H79" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I79" s="69" t="s">
+        <v>234</v>
+      </c>
+      <c r="J79" s="69" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B80" s="105" t="s">
+        <v>226</v>
+      </c>
+      <c r="C80" s="107" t="s">
+        <v>229</v>
+      </c>
+      <c r="D80" s="112" t="s">
+        <v>232</v>
+      </c>
+      <c r="E80" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F80" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G80" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H80" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I80" s="69" t="s">
+        <v>234</v>
+      </c>
+      <c r="J80" s="69" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B81" s="105" t="s">
+        <v>227</v>
+      </c>
+      <c r="C81" s="107" t="s">
+        <v>230</v>
+      </c>
+      <c r="D81" s="112" t="s">
+        <v>233</v>
+      </c>
+      <c r="E81" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F81" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G81" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="H81" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I81" s="69" t="s">
+        <v>234</v>
+      </c>
+      <c r="J81" s="69" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>